<commit_message>
Update PC script for 2022
</commit_message>
<xml_diff>
--- a/PC/Data/ScoutDataTemplate.xlsx
+++ b/PC/Data/ScoutDataTemplate.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20384"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Team100\Desktop\Qt\QRtoExcel\Shortcut\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adogg\Documents\GitHub\Scouting2018\PC\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F25365C-8C97-4E10-A30A-857A27421B4C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19368" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19365" windowHeight="9195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Initialization</t>
   </si>
@@ -30,12 +31,6 @@
     <t>Tele-Op</t>
   </si>
   <si>
-    <t>Fouls  /</t>
-  </si>
-  <si>
-    <t>Misc.</t>
-  </si>
-  <si>
     <t>Team #</t>
   </si>
   <si>
@@ -54,36 +49,6 @@
     <t>Cross Line</t>
   </si>
   <si>
-    <t>Place Cubes:</t>
-  </si>
-  <si>
-    <t>On Switch</t>
-  </si>
-  <si>
-    <t>On Scale</t>
-  </si>
-  <si>
-    <t>Pick up Cubes</t>
-  </si>
-  <si>
-    <t>Cubes in Switch</t>
-  </si>
-  <si>
-    <t>Cubes on Scale</t>
-  </si>
-  <si>
-    <t>Cubes in Exchange</t>
-  </si>
-  <si>
-    <t>Climb</t>
-  </si>
-  <si>
-    <t>Support</t>
-  </si>
-  <si>
-    <t>Share Bar</t>
-  </si>
-  <si>
     <t>Fouls</t>
   </si>
   <si>
@@ -100,13 +65,31 @@
   </si>
   <si>
     <t>Broken</t>
+  </si>
+  <si>
+    <t>High Goal</t>
+  </si>
+  <si>
+    <t>Low Goal</t>
+  </si>
+  <si>
+    <t>Climb Level</t>
+  </si>
+  <si>
+    <t>Qualitative</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Fouls  / Misc.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,8 +126,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,8 +168,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -201,36 +197,66 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="5"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="5" builtinId="23"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,142 +558,133 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
+      <selection pane="bottomLeft" activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.44140625" customWidth="1"/>
-    <col min="2" max="2" width="7.5546875" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" customWidth="1"/>
-    <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" customWidth="1"/>
-    <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="9" max="9" width="8.109375" customWidth="1"/>
-    <col min="10" max="10" width="11.77734375" customWidth="1"/>
-    <col min="11" max="11" width="13.5546875" customWidth="1"/>
-    <col min="12" max="12" width="12.77734375" customWidth="1"/>
-    <col min="13" max="13" width="15.6640625" customWidth="1"/>
-    <col min="14" max="14" width="5.21875" customWidth="1"/>
-    <col min="15" max="15" width="7.21875" customWidth="1"/>
-    <col min="16" max="16" width="9" customWidth="1"/>
-    <col min="17" max="17" width="5" customWidth="1"/>
-    <col min="18" max="18" width="9.33203125" customWidth="1"/>
-    <col min="19" max="19" width="9.88671875" customWidth="1"/>
-    <col min="20" max="20" width="8.21875" customWidth="1"/>
-    <col min="21" max="21" width="7.88671875" customWidth="1"/>
-    <col min="22" max="22" width="6.88671875" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="72.7109375" customWidth="1"/>
+    <col min="19" max="19" width="8.28515625" customWidth="1"/>
+    <col min="20" max="20" width="7.85546875" customWidth="1"/>
+    <col min="21" max="21" width="6.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5" t="s">
+    <row r="1" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="6" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="7" t="s">
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="8" t="s">
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
+    <row r="3" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="L1:Q1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
 </worksheet>

</xml_diff>